<commit_message>
updated materials, added syllabus
</commit_message>
<xml_diff>
--- a/material/data/schedule.xlsx
+++ b/material/data/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebstier/Library/CloudStorage/Dropbox/Lehrveranstaltungen/2024 - Mannheim/ma_css24/material/extra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebstier/Library/CloudStorage/Dropbox/Lehrveranstaltungen/2024 - Mannheim/ma_css24/material/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000ADDF6-53C8-404B-B64C-B3E5748BEE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA106894-16DF-154D-B443-748AE9FD9907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6C7A0B95-C424-6845-B994-5F3721DB8565}"/>
   </bookViews>
@@ -66,10 +66,6 @@
 - Linked surveys and DBD </t>
   </si>
   <si>
-    <t>- Automated text analysis 
-- Machine learning</t>
-  </si>
-  <si>
     <t>- Large Language Models 
 - Network Analysis</t>
   </si>
@@ -91,36 +87,40 @@
   </si>
   <si>
     <t>- Presentations of thesis ideas 
-- Coding troubleshooting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Open science and reproducibility in CSS
-- Data quality and validation in CSS
-- Coding repetitions
-- Something else </t>
+- Coding: troubleshooting</t>
   </si>
   <si>
     <t>Bauer, P. C., &amp; Landesvatter, C. (2023). Writing a reproducible paper with RStudio and Quarto. [*OSF Preprint*.](https://doi.org/10.31219/osf.io/ur4xn)</t>
-  </si>
-  <si>
-    <t>Grimmer, J., &amp; Stewart, B. M. (2013). Text as Data: The Promise and Pitfalls of Automatic Content Analysis Methods for Political Texts. [*Political Analysis*, 21(3), 267–297.](https://doi.org/10.1093/pan/mps028) &lt;br/&gt;&lt;br/&gt;
-Schwemmer, C., &amp; Wieczorek, O. (2020). The Methodological Divide of Sociology: Evidence from Two Decades of Journal Publications. [*Sociology*, 54(1), 3–21.](https://doi.org/10.1177/0038038519853146)</t>
   </si>
   <si>
     <t>Gilardi, F., Alizadeh, M., &amp; Kubli, M. (2023). ChatGPT outperforms crowd workers for text-annotation tasks. [*PNAS*, 120(30).](https://doi.org/10.1073/pnas.2305016120)  &lt;br/&gt;&lt;br/&gt;
 Reiss, M. V. (2023). Testing the Reliability of ChatGPT for Text Annotation and Classification: A Cautionary Remark. [*arXiv Preprint*.](http://arxiv.org/abs/2304.11085)</t>
   </si>
   <si>
-    <t>Schoch, D., Chan, C., Wagner, C., &amp; Bleier, A. (2023). Computational Reproducibility in Computational Social Science. [*arXiv Preprint*.](http://arxiv.org/abs/2307.01918) &lt;br/&gt;&lt;br/&gt;
-Sen, I., Flöck, F., Weller, K., Weiß, B., &amp; Wagner, C. (2021). A Total Error Framework for Digital Traces of Human Behavior on Online Platforms. [*Public Opinion Quarterly*, 85(S1), 399–422.](https://doi.org/10.1093/poq/nfab018)</t>
-  </si>
-  <si>
     <t>Guess, A. M., Barberá, P., Munzert, S., &amp; Yang, J. (2021). The consequences of online partisan media. [*PNAS*, 118(14).](https://doi.org/10.1073/pnas.2013464118) &lt;br/&gt;&lt;br/&gt;
 Silber, H., Breuer, J., Beuthner, C., Gummer, T., Keusch, F., Siegers, P., Stier, S., &amp; Weiß, B. (2022). Linking Surveys and Digital Trace Data: Insights From two Studies on Determinants of Data Sharing Behaviour. [*Journal of the Royal Statistical Society Series A: Statistics in Society*, 185(S2), S387–S407.](https://doi.org/10.1111/rssa.12954)</t>
   </si>
   <si>
     <t>Fiesler, C., &amp; Proferes, N. (2018). 'Participant' Perceptions of Twitter Research Ethics. [*Social Media + Society*, 4(1).](https://doi.org/10.1177/2056305118763366) &lt;br/&gt;&lt;br/&gt;
 Freelon, D. (2018). Computational Research in the Post-API Age. [*Political Communication*, 35(4), 665–668.](https://osf.io/preprints/socarxiv/56f4q)</t>
+  </si>
+  <si>
+    <t>Bonikowski, B., Luo, Y., &amp; Stuhler, O. (2022). Politics as Usual? Measuring Populism, Nationalism, and Authoritarianism in U.S. Presidential Campaigns (1952–2020) with Neural Language Models. [*Sociological Methods &amp; Research*, 51(4), 1721–1787.](https://doi.org/10.31235/osf.io/uhvbp) &lt;br/&gt;&lt;br/&gt;
+Schwemmer, C., &amp; Wieczorek, O. (2020). The Methodological Divide of Sociology: Evidence from Two Decades of Journal Publications. [*Sociology*, 54(1), 3–21.](https://doi.org/10.1177/0038038519853146)</t>
+  </si>
+  <si>
+    <t>- Automated text analysis 
+- Supervised and unsupervised models
+- Machine learning</t>
+  </si>
+  <si>
+    <t>- Open science and reproducibility in CSS
+- Data quality and validation in CSS
+- Coding: open questions</t>
+  </si>
+  <si>
+    <t>Chan, C., Schatto-Eckrodt, T., &amp; Gruber, J. B. (2024). What makes computational communication science (ir)reproducible? [*Working Paper*.](material/data/chan_et_al.pdf) &lt;br/&gt;&lt;br/&gt;
+Nyhan, B., Settle, J., Thorson, E., Wojcieszak, M., Barberá, P., et al. (2023). Like-minded sources on Facebook are prevalent but not polarizing. [*Nature*, 620(7972), 137–144.](https://doi.org/10.1038/s41586-023-06297-w)</t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C1A341-8F6A-B141-BAE2-758F9533CD08}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -519,7 +519,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="85">
@@ -530,10 +530,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="230" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="155" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -541,29 +541,29 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="181" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="119">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="119">
@@ -571,10 +571,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34">
@@ -582,10 +582,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>